<commit_message>
Xong các chức năng cơ bản yêu cầu
</commit_message>
<xml_diff>
--- a/DB_QUANLYNHANSU.xlsx
+++ b/DB_QUANLYNHANSU.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Thực tập nhóm_TH13\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Thực tập nhóm_TH13\BaiTapLon\QuanlynhansuTSM\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="38">
   <si>
     <t>Nhomquyen (Nhóm quyền )</t>
   </si>
@@ -136,6 +136,9 @@
   </si>
   <si>
     <t>datetime</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -1685,14 +1688,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="L35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="L35" sqref="L35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="35" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L35" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>